<commit_message>
update for svg image, extract positions from svg object
</commit_message>
<xml_diff>
--- a/Source/Pokerface/wwwroot/images/PosCalculation.xlsx
+++ b/Source/Pokerface/wwwroot/images/PosCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vs_workspace\C#\Blazor Pokerface\Source\Pokerface\wwwroot\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F69BA4-D4D2-4AF1-8F0E-EC6371202BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D206D63-6E8B-455E-B0D0-434E5ED4690A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FAF6CB02-F6BB-431E-A497-149C9B9A438F}"/>
   </bookViews>
@@ -500,9 +500,9 @@
   <dimension ref="C3:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,10 +534,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>36</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="E5" s="1">
-        <v>54</v>
+        <v>54.3</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.35">
@@ -570,11 +570,11 @@
       </c>
       <c r="D10">
         <f>$D$7-2*$D$8-2.5*$D$5</f>
-        <v>290</v>
+        <v>289.25</v>
       </c>
       <c r="E10">
         <f>$E$7-$E$5/2</f>
-        <v>223</v>
+        <v>222.85</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.35">
@@ -583,11 +583,11 @@
       </c>
       <c r="D11">
         <f>D10+$D$5+$D$8</f>
-        <v>336</v>
+        <v>335.55</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E14" si="0">$E$7-$E$5/2</f>
-        <v>223</v>
+        <v>222.85</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.35">
@@ -596,11 +596,11 @@
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D14" si="1">D11+$D$5+$D$8</f>
-        <v>382</v>
+        <v>381.85</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>223</v>
+        <v>222.85</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.35">
@@ -609,11 +609,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>428</v>
+        <v>428.15000000000003</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>223</v>
+        <v>222.85</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.35">
@@ -622,11 +622,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>474</v>
+        <v>474.45000000000005</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>223</v>
+        <v>222.85</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.35">
@@ -647,7 +647,7 @@
       </c>
       <c r="E18">
         <f>$E$7-$E$8/2-$D$5</f>
-        <v>209</v>
+        <v>208.7</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
@@ -669,11 +669,11 @@
       </c>
       <c r="D21">
         <f>$D$4-$D$17-$E$5</f>
-        <v>691</v>
+        <v>690.7</v>
       </c>
       <c r="E21">
         <f>E18</f>
-        <v>209</v>
+        <v>208.7</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.35">
@@ -682,7 +682,7 @@
       </c>
       <c r="D22">
         <f>D21</f>
-        <v>691</v>
+        <v>690.7</v>
       </c>
       <c r="E22">
         <f>E21+10+$D$5</f>
@@ -694,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="D24">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.35">
@@ -711,7 +711,7 @@
       </c>
       <c r="D27">
         <f>$D$7-$D$8/2-$D$5</f>
-        <v>359</v>
+        <v>358.7</v>
       </c>
       <c r="E27">
         <f>$E$25</f>
@@ -737,7 +737,7 @@
       </c>
       <c r="D30">
         <f>D27-$D$24-$D$5</f>
-        <v>238</v>
+        <v>242.39999999999998</v>
       </c>
       <c r="E30">
         <f>$E$25</f>
@@ -750,7 +750,7 @@
       </c>
       <c r="D31">
         <f>D30-$D$8-$D$5</f>
-        <v>192</v>
+        <v>196.09999999999997</v>
       </c>
       <c r="E31">
         <f>$E$25</f>
@@ -763,7 +763,7 @@
       </c>
       <c r="D33">
         <f>D28+$D$24+$D$5</f>
-        <v>526</v>
+        <v>521.29999999999995</v>
       </c>
       <c r="E33">
         <f>$E$25</f>
@@ -776,7 +776,7 @@
       </c>
       <c r="D34">
         <f>D33+$D$8+$D$5</f>
-        <v>572</v>
+        <v>567.59999999999991</v>
       </c>
       <c r="E34">
         <f>$E$25</f>
@@ -789,11 +789,11 @@
       </c>
       <c r="D37">
         <f>D27</f>
-        <v>359</v>
+        <v>358.7</v>
       </c>
       <c r="E37">
         <f>$E$4-$E$25-$E$5</f>
-        <v>396</v>
+        <v>395.7</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
@@ -806,7 +806,7 @@
       </c>
       <c r="E38">
         <f t="shared" ref="E38:E44" si="3">$E$4-$E$25-$E$5</f>
-        <v>396</v>
+        <v>395.7</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.35">
@@ -815,11 +815,11 @@
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
-        <v>238</v>
+        <v>242.39999999999998</v>
       </c>
       <c r="E40">
         <f t="shared" si="3"/>
-        <v>396</v>
+        <v>395.7</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.35">
@@ -828,11 +828,11 @@
       </c>
       <c r="D41">
         <f t="shared" si="2"/>
-        <v>192</v>
+        <v>196.09999999999997</v>
       </c>
       <c r="E41">
         <f t="shared" si="3"/>
-        <v>396</v>
+        <v>395.7</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.35">
@@ -841,11 +841,11 @@
       </c>
       <c r="D43">
         <f t="shared" si="2"/>
-        <v>526</v>
+        <v>521.29999999999995</v>
       </c>
       <c r="E43">
         <f t="shared" si="3"/>
-        <v>396</v>
+        <v>395.7</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.35">
@@ -854,11 +854,11 @@
       </c>
       <c r="D44">
         <f t="shared" si="2"/>
-        <v>572</v>
+        <v>567.59999999999991</v>
       </c>
       <c r="E44">
         <f t="shared" si="3"/>
-        <v>396</v>
+        <v>395.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>